<commit_message>
added distinctive collexeme analysis
</commit_message>
<xml_diff>
--- a/data/overview_tables/distinctive_collexeme_analysis_overview.xlsx
+++ b/data/overview_tables/distinctive_collexeme_analysis_overview.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanhartmann/sciebo/Tutorials/collostructions_tutorial/data/overview_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245D7CF8-DE79-6542-BF73-3711293313B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F53011B-9687-0B43-8267-F84BFEA645FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14180" xr2:uid="{9C19626E-32DE-0E4E-8797-5F6FA71A0C76}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14180" activeTab="1" xr2:uid="{9C19626E-32DE-0E4E-8797-5F6FA71A0C76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -23,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Total</t>
   </si>
@@ -76,6 +75,33 @@
   </si>
   <si>
     <t>Construction c₂ of Class C</t>
+  </si>
+  <si>
+    <t>Frequency of all other nouns in the "mother of all" cxn</t>
+  </si>
+  <si>
+    <t>Frequency of "hangover" in the "ADJ-est N ever" construction</t>
+  </si>
+  <si>
+    <t>Frequency of "hangover" in the "mother of all" cxn</t>
+  </si>
+  <si>
+    <t>Frequency of all other nouns in the "ADJ-est N ever" construction</t>
+  </si>
+  <si>
+    <t>Total frequency of "hangover" in both constructions</t>
+  </si>
+  <si>
+    <t>Total frequency of all other nouns in the two constructions</t>
+  </si>
+  <si>
+    <t>Total frequency of "mother of all"</t>
+  </si>
+  <si>
+    <t>Total frequency of "ADJ-est N ever"</t>
+  </si>
+  <si>
+    <t>Total frequency of both cxns</t>
   </si>
 </sst>
 </file>
@@ -436,14 +462,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F7D6EA-6AA2-0A41-8FE2-D79AE3C1AD2A}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="76.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -524,4 +551,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE33280-D995-974A-A9F6-2CCCECFBF3F6}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="48.83203125" customWidth="1"/>
+    <col min="3" max="3" width="45.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>